<commit_message>
Generate excel file using template
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/single.xlsx
+++ b/src/main/resources/templates/single.xlsx
@@ -23,9 +23,59 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>Postes/occupants</t>
+  </si>
+  <si>
+    <t>Date de Prise de Fonction</t>
+  </si>
+  <si>
+    <t>Anciennete</t>
+  </si>
+  <si>
+    <t>Potentiel d'Evolution</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Statut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Décision Talent Management </t>
+  </si>
+  <si>
+    <t>Revalorisatoion</t>
+  </si>
+  <si>
+    <t>Promotion</t>
+  </si>
+  <si>
+    <t>Prime Exceptionnelle</t>
+  </si>
+  <si>
+    <t>Autres Avantages</t>
+  </si>
+  <si>
+    <t>Formations</t>
+  </si>
+  <si>
+    <t>Action Suivi pour 2024</t>
+  </si>
+  <si>
+    <t>Commentaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">People Review </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,16 +83,68 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -50,12 +152,234 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,12 +660,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:O2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="2"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="2">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+    </row>
+    <row r="3" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="2:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="17"/>
+    </row>
+    <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="10"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:O4"/>
+    <mergeCell ref="N5:O5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>